<commit_message>
processing time graph added
</commit_message>
<xml_diff>
--- a/Analysis/Analysis.xlsx
+++ b/Analysis/Analysis.xlsx
@@ -307,7 +307,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -450,7 +449,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -553,7 +551,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -665,7 +662,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -844,6 +840,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -941,7 +938,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -963,7 +962,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -985,7 +986,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1147,7 +1150,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1169,7 +1174,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1209,6 +1216,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1308,7 +1316,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1330,7 +1340,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1352,7 +1364,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-C446-4A85-9AE3-510A46E0AA63}"/>
                 </c:ext>
@@ -1617,6 +1631,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2478,7 +2493,7 @@
                 </a:solidFill>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Time Analysis</a:t>
+              <a:t>Processing Time Analysis</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3006,9 +3021,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3030,9 +3043,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3054,9 +3065,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3200,9 +3209,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3224,9 +3231,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3271,7 +3276,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3371,9 +3375,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3395,9 +3397,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3419,9 +3419,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-68A1-4C11-ADE8-830CCE577472}"/>
                 </c:ext>
@@ -3918,7 +3916,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4016,9 +4013,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-F02D-4575-8DF3-EC06E0BB6067}"/>
                 </c:ext>
@@ -4040,9 +4035,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-F02D-4575-8DF3-EC06E0BB6067}"/>
                 </c:ext>
@@ -4084,7 +4077,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4207,9 +4199,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-F02D-4575-8DF3-EC06E0BB6067}"/>
                 </c:ext>
@@ -4251,7 +4241,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4351,9 +4340,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-F02D-4575-8DF3-EC06E0BB6067}"/>
                 </c:ext>
@@ -4375,9 +4362,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-F02D-4575-8DF3-EC06E0BB6067}"/>
                 </c:ext>
@@ -4419,7 +4404,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4527,7 +4511,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4641,7 +4624,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4710,7 +4692,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4816,7 +4797,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4914,9 +4894,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -4938,9 +4916,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -4962,9 +4938,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5128,9 +5102,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5152,9 +5124,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5196,7 +5166,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5296,9 +5265,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5320,9 +5287,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5344,9 +5309,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-8715-4EA8-BCFE-BEE3CC5BD7FC}"/>
                 </c:ext>
@@ -5619,7 +5582,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5803,7 +5765,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5901,9 +5862,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-1988-46D7-8396-27614CA7F775}"/>
                 </c:ext>
@@ -5925,9 +5884,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-1988-46D7-8396-27614CA7F775}"/>
                 </c:ext>
@@ -5969,7 +5926,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6092,9 +6048,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-1988-46D7-8396-27614CA7F775}"/>
                 </c:ext>
@@ -6136,7 +6090,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6236,9 +6189,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-1988-46D7-8396-27614CA7F775}"/>
                 </c:ext>
@@ -6260,9 +6211,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-1988-46D7-8396-27614CA7F775}"/>
                 </c:ext>
@@ -6304,7 +6253,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6412,7 +6360,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6529,7 +6476,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6711,7 +6657,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6844,7 +6789,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6971,7 +6915,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16579,16 +16522,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>17438</xdr:colOff>
-      <xdr:row>258</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>407963</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>292</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17223,8 +17166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D256" workbookViewId="0">
-      <selection activeCell="Y279" sqref="Y279"/>
+    <sheetView tabSelected="1" topLeftCell="D268" workbookViewId="0">
+      <selection activeCell="Z278" sqref="Z278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>